<commit_message>
Use new sample xml file
</commit_message>
<xml_diff>
--- a/liiatools/spec/social_work_workforce/samples/request/pivotTable.xlsx
+++ b/liiatools/spec/social_work_workforce/samples/request/pivotTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>FTESum</t>
   </si>
@@ -32,6 +32,27 @@
   </si>
   <si>
     <t>Ethnicity_Compact</t>
+  </si>
+  <si>
+    <t>Barking and Dagenham</t>
+  </si>
+  <si>
+    <t>Not known (gender has not been recorded)</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>not specified (indeterminate; unable to be classified as either male or female)</t>
+  </si>
+  <si>
+    <t>Declared not stated or Refused</t>
+  </si>
+  <si>
+    <t>White and Asian</t>
+  </si>
+  <si>
+    <t>Any Other White Background</t>
   </si>
 </sst>
 </file>
@@ -389,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -415,6 +436,86 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>0.192894</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>0.786453</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>0.521371</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>